<commit_message>
expand and test DynamicModel
</commit_message>
<xml_diff>
--- a/tests/fixtures/Mycoplasma pneumoniae.xlsx
+++ b/tests/fixtures/Mycoplasma pneumoniae.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_sim/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="24780" windowHeight="15560" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -22,8 +27,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Species!$A$1:$L$147</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Submodels!$A$1:$C$5</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -3829,7 +3837,7 @@
       <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -3837,7 +3845,7 @@
     <col min="4" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3848,7 +3856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -3859,7 +3867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -3870,7 +3878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -3881,7 +3889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -3895,11 +3903,6 @@
   </sheetData>
   <autoFilter ref="A1:C5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3914,7 +3917,7 @@
       <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
@@ -3923,7 +3926,7 @@
     <col min="5" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3937,7 +3940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -3951,7 +3954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -3968,11 +3971,6 @@
   </sheetData>
   <autoFilter ref="A1:D3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3981,13 +3979,13 @@
   <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="8.83203125" style="3"/>
     <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
@@ -4001,7 +3999,7 @@
     <col min="13" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="45" customHeight="1">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4039,7 +4037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>267</v>
       </c>
@@ -4060,7 +4058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>269</v>
       </c>
@@ -4076,7 +4074,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -4094,7 +4092,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>270</v>
       </c>
@@ -4115,7 +4113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -4133,7 +4131,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -4151,7 +4149,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>272</v>
       </c>
@@ -4172,7 +4170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -4190,7 +4188,7 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>274</v>
       </c>
@@ -4211,7 +4209,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1">
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -4229,7 +4227,7 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>276</v>
       </c>
@@ -4250,7 +4248,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -4268,7 +4266,7 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>278</v>
       </c>
@@ -4284,7 +4282,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -4302,7 +4300,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>279</v>
       </c>
@@ -4323,7 +4321,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1">
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4341,7 +4339,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1">
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
@@ -4359,7 +4357,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>284</v>
       </c>
@@ -4380,7 +4378,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>282</v>
       </c>
@@ -4401,7 +4399,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>286</v>
       </c>
@@ -4417,7 +4415,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>288</v>
       </c>
@@ -4433,7 +4431,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>290</v>
       </c>
@@ -4449,7 +4447,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>292</v>
       </c>
@@ -4465,7 +4463,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1">
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>294</v>
       </c>
@@ -4481,7 +4479,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1">
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>296</v>
       </c>
@@ -4497,7 +4495,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>298</v>
       </c>
@@ -4513,7 +4511,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -4531,7 +4529,7 @@
       </c>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>300</v>
       </c>
@@ -4552,7 +4550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>55</v>
       </c>
@@ -4570,7 +4568,7 @@
       </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>305</v>
       </c>
@@ -4591,7 +4589,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
@@ -4609,7 +4607,7 @@
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1">
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>307</v>
       </c>
@@ -4630,7 +4628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1">
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
@@ -4648,7 +4646,7 @@
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1">
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>309</v>
       </c>
@@ -4669,7 +4667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1">
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
@@ -4687,7 +4685,7 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1">
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>302</v>
       </c>
@@ -4708,7 +4706,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1">
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
@@ -4726,7 +4724,7 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1">
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -4749,7 +4747,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1">
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>43</v>
       </c>
@@ -4772,7 +4770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1">
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>61</v>
       </c>
@@ -4790,7 +4788,7 @@
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1">
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>311</v>
       </c>
@@ -4811,7 +4809,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1">
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>63</v>
       </c>
@@ -4829,7 +4827,7 @@
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1">
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>313</v>
       </c>
@@ -4850,7 +4848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1">
+    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>315</v>
       </c>
@@ -4866,7 +4864,7 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1">
+    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>65</v>
       </c>
@@ -4884,7 +4882,7 @@
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:12" ht="15" customHeight="1">
+    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>317</v>
       </c>
@@ -4905,7 +4903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1">
+    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>67</v>
       </c>
@@ -4923,7 +4921,7 @@
       </c>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:12" ht="15" customHeight="1">
+    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>319</v>
       </c>
@@ -4944,7 +4942,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15" customHeight="1">
+    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
@@ -4962,7 +4960,7 @@
       </c>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" spans="1:12" ht="15" customHeight="1">
+    <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>321</v>
       </c>
@@ -4983,7 +4981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15" customHeight="1">
+    <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>323</v>
       </c>
@@ -5004,7 +5002,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15" customHeight="1">
+    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>325</v>
       </c>
@@ -5020,7 +5018,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
     </row>
-    <row r="54" spans="1:12" ht="15" customHeight="1">
+    <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>327</v>
       </c>
@@ -5041,7 +5039,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1">
+    <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>330</v>
       </c>
@@ -5057,7 +5055,7 @@
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" spans="1:12" ht="15" customHeight="1">
+    <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>71</v>
       </c>
@@ -5075,7 +5073,7 @@
       </c>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="1:12" ht="15" customHeight="1">
+    <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>340</v>
       </c>
@@ -5096,7 +5094,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15" customHeight="1">
+    <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>41</v>
       </c>
@@ -5119,7 +5117,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15" customHeight="1">
+    <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>332</v>
       </c>
@@ -5140,7 +5138,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15" customHeight="1">
+    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>40</v>
       </c>
@@ -5158,7 +5156,7 @@
       </c>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="1:12" ht="15" customHeight="1">
+    <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>334</v>
       </c>
@@ -5174,7 +5172,7 @@
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" spans="1:12" ht="15" customHeight="1">
+    <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>73</v>
       </c>
@@ -5192,7 +5190,7 @@
       </c>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" spans="1:12" ht="15" customHeight="1">
+    <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>342</v>
       </c>
@@ -5213,7 +5211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15" customHeight="1">
+    <row r="64" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>336</v>
       </c>
@@ -5229,7 +5227,7 @@
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="1:12" ht="15" customHeight="1">
+    <row r="65" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>338</v>
       </c>
@@ -5245,7 +5243,7 @@
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="1:12" ht="15" customHeight="1">
+    <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>344</v>
       </c>
@@ -5261,7 +5259,7 @@
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" spans="1:12" ht="15" customHeight="1">
+    <row r="67" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>346</v>
       </c>
@@ -5277,7 +5275,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:12" ht="15" customHeight="1">
+    <row r="68" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>348</v>
       </c>
@@ -5293,7 +5291,7 @@
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" spans="1:12" ht="15" customHeight="1">
+    <row r="69" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>75</v>
       </c>
@@ -5311,7 +5309,7 @@
       </c>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" spans="1:12" ht="15" customHeight="1">
+    <row r="70" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>350</v>
       </c>
@@ -5332,7 +5330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15" customHeight="1">
+    <row r="71" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>352</v>
       </c>
@@ -5348,7 +5346,7 @@
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" spans="1:12" ht="15" customHeight="1">
+    <row r="72" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>354</v>
       </c>
@@ -5364,7 +5362,7 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="1:12" ht="15" customHeight="1">
+    <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>77</v>
       </c>
@@ -5382,7 +5380,7 @@
       </c>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:12" ht="15" customHeight="1">
+    <row r="74" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>356</v>
       </c>
@@ -5403,7 +5401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15" customHeight="1">
+    <row r="75" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>79</v>
       </c>
@@ -5421,7 +5419,7 @@
       </c>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:12" ht="15" customHeight="1">
+    <row r="76" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>358</v>
       </c>
@@ -5442,7 +5440,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15" customHeight="1">
+    <row r="77" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>81</v>
       </c>
@@ -5460,7 +5458,7 @@
       </c>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="1:12" ht="15" customHeight="1">
+    <row r="78" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>360</v>
       </c>
@@ -5481,7 +5479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15" customHeight="1">
+    <row r="79" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>362</v>
       </c>
@@ -5497,7 +5495,7 @@
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="1:12" ht="15" customHeight="1">
+    <row r="80" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>37</v>
       </c>
@@ -5515,7 +5513,7 @@
       </c>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" spans="1:12" ht="15" customHeight="1">
+    <row r="81" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>363</v>
       </c>
@@ -5536,7 +5534,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15" customHeight="1">
+    <row r="82" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>366</v>
       </c>
@@ -5552,7 +5550,7 @@
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" spans="1:12" ht="15" customHeight="1">
+    <row r="83" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>31</v>
       </c>
@@ -5575,7 +5573,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15" customHeight="1">
+    <row r="84" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
@@ -5593,7 +5591,7 @@
       </c>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="1:12" ht="15" customHeight="1">
+    <row r="85" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>368</v>
       </c>
@@ -5614,7 +5612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15" customHeight="1">
+    <row r="86" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>370</v>
       </c>
@@ -5629,7 +5627,7 @@
       </c>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:12" ht="15" customHeight="1">
+    <row r="87" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>95</v>
       </c>
@@ -5650,7 +5648,7 @@
       </c>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="1:12" ht="15" customHeight="1">
+    <row r="88" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>98</v>
       </c>
@@ -5671,7 +5669,7 @@
       </c>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="1:12" ht="15" customHeight="1">
+    <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>101</v>
       </c>
@@ -5692,7 +5690,7 @@
       </c>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" spans="1:12" ht="15" customHeight="1">
+    <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>104</v>
       </c>
@@ -5713,7 +5711,7 @@
       </c>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="1:12" ht="15" customHeight="1">
+    <row r="91" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>107</v>
       </c>
@@ -5734,7 +5732,7 @@
       </c>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:12" ht="15" customHeight="1">
+    <row r="92" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>110</v>
       </c>
@@ -5755,7 +5753,7 @@
       </c>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="1:12" ht="15" customHeight="1">
+    <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>116</v>
       </c>
@@ -5776,7 +5774,7 @@
       </c>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="1:12" ht="15" customHeight="1">
+    <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>119</v>
       </c>
@@ -5797,7 +5795,7 @@
       </c>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="1:12" ht="15" customHeight="1">
+    <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>149</v>
       </c>
@@ -5818,7 +5816,7 @@
       </c>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="1:12" ht="15" customHeight="1">
+    <row r="96" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>122</v>
       </c>
@@ -5839,7 +5837,7 @@
       </c>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="1:9" ht="15" customHeight="1">
+    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>125</v>
       </c>
@@ -5860,7 +5858,7 @@
       </c>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" spans="1:9" ht="15" customHeight="1">
+    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>173</v>
       </c>
@@ -5881,7 +5879,7 @@
       </c>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9" ht="15" customHeight="1">
+    <row r="99" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>128</v>
       </c>
@@ -5902,7 +5900,7 @@
       </c>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9" ht="15" customHeight="1">
+    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>131</v>
       </c>
@@ -5923,7 +5921,7 @@
       </c>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="1:9" ht="15" customHeight="1">
+    <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>134</v>
       </c>
@@ -5944,7 +5942,7 @@
       </c>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="1:9" ht="15" customHeight="1">
+    <row r="102" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>113</v>
       </c>
@@ -5965,7 +5963,7 @@
       </c>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="1:9" ht="15" customHeight="1">
+    <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>170</v>
       </c>
@@ -5986,7 +5984,7 @@
       </c>
       <c r="I103" s="4"/>
     </row>
-    <row r="104" spans="1:9" ht="15" customHeight="1">
+    <row r="104" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>137</v>
       </c>
@@ -6007,7 +6005,7 @@
       </c>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:9" ht="15" customHeight="1">
+    <row r="105" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>140</v>
       </c>
@@ -6028,7 +6026,7 @@
       </c>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="1:9" ht="15" customHeight="1">
+    <row r="106" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>167</v>
       </c>
@@ -6049,7 +6047,7 @@
       </c>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="1:9" ht="15" customHeight="1">
+    <row r="107" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>143</v>
       </c>
@@ -6070,7 +6068,7 @@
       </c>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:9" ht="15" customHeight="1">
+    <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>161</v>
       </c>
@@ -6091,7 +6089,7 @@
       </c>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" spans="1:9" ht="15" customHeight="1">
+    <row r="109" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>89</v>
       </c>
@@ -6112,7 +6110,7 @@
       </c>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" spans="1:9" ht="15" customHeight="1">
+    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>85</v>
       </c>
@@ -6133,7 +6131,7 @@
       </c>
       <c r="I110" s="4"/>
     </row>
-    <row r="111" spans="1:9" ht="15" customHeight="1">
+    <row r="111" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>92</v>
       </c>
@@ -6154,7 +6152,7 @@
       </c>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" spans="1:9" ht="15" customHeight="1">
+    <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>146</v>
       </c>
@@ -6175,7 +6173,7 @@
       </c>
       <c r="I112" s="4"/>
     </row>
-    <row r="113" spans="1:9" ht="15" customHeight="1">
+    <row r="113" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>152</v>
       </c>
@@ -6196,7 +6194,7 @@
       </c>
       <c r="I113" s="4"/>
     </row>
-    <row r="114" spans="1:9" ht="15" customHeight="1">
+    <row r="114" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>155</v>
       </c>
@@ -6217,7 +6215,7 @@
       </c>
       <c r="I114" s="4"/>
     </row>
-    <row r="115" spans="1:9" ht="15" customHeight="1">
+    <row r="115" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>158</v>
       </c>
@@ -6238,7 +6236,7 @@
       </c>
       <c r="I115" s="4"/>
     </row>
-    <row r="116" spans="1:9" ht="15" customHeight="1">
+    <row r="116" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>164</v>
       </c>
@@ -6259,7 +6257,7 @@
       </c>
       <c r="I116" s="4"/>
     </row>
-    <row r="117" spans="1:9" ht="15" customHeight="1">
+    <row r="117" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>186</v>
       </c>
@@ -6280,7 +6278,7 @@
       </c>
       <c r="I117" s="4"/>
     </row>
-    <row r="118" spans="1:9" ht="15" customHeight="1">
+    <row r="118" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>189</v>
       </c>
@@ -6301,7 +6299,7 @@
       </c>
       <c r="I118" s="4"/>
     </row>
-    <row r="119" spans="1:9" ht="15" customHeight="1">
+    <row r="119" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>192</v>
       </c>
@@ -6322,7 +6320,7 @@
       </c>
       <c r="I119" s="4"/>
     </row>
-    <row r="120" spans="1:9" ht="15" customHeight="1">
+    <row r="120" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>195</v>
       </c>
@@ -6343,7 +6341,7 @@
       </c>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="1:9" ht="15" customHeight="1">
+    <row r="121" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>198</v>
       </c>
@@ -6364,7 +6362,7 @@
       </c>
       <c r="I121" s="4"/>
     </row>
-    <row r="122" spans="1:9" ht="15" customHeight="1">
+    <row r="122" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>201</v>
       </c>
@@ -6385,7 +6383,7 @@
       </c>
       <c r="I122" s="4"/>
     </row>
-    <row r="123" spans="1:9" ht="15" customHeight="1">
+    <row r="123" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>207</v>
       </c>
@@ -6406,7 +6404,7 @@
       </c>
       <c r="I123" s="4"/>
     </row>
-    <row r="124" spans="1:9" ht="15" customHeight="1">
+    <row r="124" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>210</v>
       </c>
@@ -6427,7 +6425,7 @@
       </c>
       <c r="I124" s="4"/>
     </row>
-    <row r="125" spans="1:9" ht="15" customHeight="1">
+    <row r="125" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>240</v>
       </c>
@@ -6448,7 +6446,7 @@
       </c>
       <c r="I125" s="4"/>
     </row>
-    <row r="126" spans="1:9" ht="15" customHeight="1">
+    <row r="126" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>213</v>
       </c>
@@ -6469,7 +6467,7 @@
       </c>
       <c r="I126" s="4"/>
     </row>
-    <row r="127" spans="1:9" ht="15" customHeight="1">
+    <row r="127" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>216</v>
       </c>
@@ -6490,7 +6488,7 @@
       </c>
       <c r="I127" s="4"/>
     </row>
-    <row r="128" spans="1:9" ht="15" customHeight="1">
+    <row r="128" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>264</v>
       </c>
@@ -6511,7 +6509,7 @@
       </c>
       <c r="I128" s="4"/>
     </row>
-    <row r="129" spans="1:9" ht="15" customHeight="1">
+    <row r="129" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>219</v>
       </c>
@@ -6532,7 +6530,7 @@
       </c>
       <c r="I129" s="4"/>
     </row>
-    <row r="130" spans="1:9" ht="15" customHeight="1">
+    <row r="130" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>222</v>
       </c>
@@ -6553,7 +6551,7 @@
       </c>
       <c r="I130" s="4"/>
     </row>
-    <row r="131" spans="1:9" ht="15" customHeight="1">
+    <row r="131" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>225</v>
       </c>
@@ -6574,7 +6572,7 @@
       </c>
       <c r="I131" s="4"/>
     </row>
-    <row r="132" spans="1:9" ht="15" customHeight="1">
+    <row r="132" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>204</v>
       </c>
@@ -6595,7 +6593,7 @@
       </c>
       <c r="I132" s="4"/>
     </row>
-    <row r="133" spans="1:9" ht="15" customHeight="1">
+    <row r="133" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>261</v>
       </c>
@@ -6616,7 +6614,7 @@
       </c>
       <c r="I133" s="4"/>
     </row>
-    <row r="134" spans="1:9" ht="15" customHeight="1">
+    <row r="134" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>228</v>
       </c>
@@ -6637,7 +6635,7 @@
       </c>
       <c r="I134" s="4"/>
     </row>
-    <row r="135" spans="1:9" ht="15" customHeight="1">
+    <row r="135" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>231</v>
       </c>
@@ -6658,7 +6656,7 @@
       </c>
       <c r="I135" s="4"/>
     </row>
-    <row r="136" spans="1:9" ht="15" customHeight="1">
+    <row r="136" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>258</v>
       </c>
@@ -6679,7 +6677,7 @@
       </c>
       <c r="I136" s="4"/>
     </row>
-    <row r="137" spans="1:9" ht="15" customHeight="1">
+    <row r="137" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>234</v>
       </c>
@@ -6700,7 +6698,7 @@
       </c>
       <c r="I137" s="4"/>
     </row>
-    <row r="138" spans="1:9" ht="15" customHeight="1">
+    <row r="138" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>252</v>
       </c>
@@ -6721,7 +6719,7 @@
       </c>
       <c r="I138" s="4"/>
     </row>
-    <row r="139" spans="1:9" ht="15" customHeight="1">
+    <row r="139" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>180</v>
       </c>
@@ -6742,7 +6740,7 @@
       </c>
       <c r="I139" s="4"/>
     </row>
-    <row r="140" spans="1:9" ht="15" customHeight="1">
+    <row r="140" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>176</v>
       </c>
@@ -6763,7 +6761,7 @@
       </c>
       <c r="I140" s="4"/>
     </row>
-    <row r="141" spans="1:9" ht="15" customHeight="1">
+    <row r="141" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>183</v>
       </c>
@@ -6784,7 +6782,7 @@
       </c>
       <c r="I141" s="4"/>
     </row>
-    <row r="142" spans="1:9" ht="15" customHeight="1">
+    <row r="142" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>237</v>
       </c>
@@ -6805,7 +6803,7 @@
       </c>
       <c r="I142" s="4"/>
     </row>
-    <row r="143" spans="1:9" ht="15" customHeight="1">
+    <row r="143" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>243</v>
       </c>
@@ -6826,7 +6824,7 @@
       </c>
       <c r="I143" s="4"/>
     </row>
-    <row r="144" spans="1:9" ht="15" customHeight="1">
+    <row r="144" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>246</v>
       </c>
@@ -6847,7 +6845,7 @@
       </c>
       <c r="I144" s="4"/>
     </row>
-    <row r="145" spans="1:9" ht="15" customHeight="1">
+    <row r="145" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>249</v>
       </c>
@@ -6868,7 +6866,7 @@
       </c>
       <c r="I145" s="4"/>
     </row>
-    <row r="146" spans="1:9" ht="15" customHeight="1">
+    <row r="146" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>255</v>
       </c>
@@ -6889,7 +6887,7 @@
       </c>
       <c r="I146" s="4"/>
     </row>
-    <row r="147" spans="1:9" ht="15" customHeight="1">
+    <row r="147" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>372</v>
       </c>
@@ -6903,11 +6901,6 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6916,13 +6909,13 @@
   <dimension ref="A1:K177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A177" sqref="A1:A177"/>
+      <selection pane="bottomRight" activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="3"/>
     <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
@@ -6937,7 +6930,7 @@
     <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="45" customHeight="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6972,7 +6965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>606</v>
       </c>
@@ -6986,7 +6979,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>379</v>
       </c>
@@ -7012,7 +7005,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>384</v>
       </c>
@@ -7029,7 +7022,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>618</v>
       </c>
@@ -7046,7 +7039,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>387</v>
       </c>
@@ -7063,7 +7056,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>621</v>
       </c>
@@ -7080,7 +7073,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>624</v>
       </c>
@@ -7097,7 +7090,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>627</v>
       </c>
@@ -7114,7 +7107,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>390</v>
       </c>
@@ -7140,7 +7133,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>597</v>
       </c>
@@ -7154,7 +7147,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>630</v>
       </c>
@@ -7171,7 +7164,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>609</v>
       </c>
@@ -7185,7 +7178,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>395</v>
       </c>
@@ -7199,7 +7192,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>398</v>
       </c>
@@ -7213,7 +7206,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>401</v>
       </c>
@@ -7227,7 +7220,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>404</v>
       </c>
@@ -7241,7 +7234,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>407</v>
       </c>
@@ -7255,7 +7248,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>410</v>
       </c>
@@ -7269,7 +7262,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>413</v>
       </c>
@@ -7283,7 +7276,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>416</v>
       </c>
@@ -7297,7 +7290,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>419</v>
       </c>
@@ -7311,7 +7304,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>422</v>
       </c>
@@ -7325,7 +7318,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>425</v>
       </c>
@@ -7339,7 +7332,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>428</v>
       </c>
@@ -7353,7 +7346,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>431</v>
       </c>
@@ -7367,7 +7360,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>434</v>
       </c>
@@ -7381,7 +7374,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>437</v>
       </c>
@@ -7395,7 +7388,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>440</v>
       </c>
@@ -7409,7 +7402,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>443</v>
       </c>
@@ -7423,7 +7416,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>446</v>
       </c>
@@ -7437,7 +7430,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>449</v>
       </c>
@@ -7451,7 +7444,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>452</v>
       </c>
@@ -7465,7 +7458,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>455</v>
       </c>
@@ -7491,7 +7484,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>460</v>
       </c>
@@ -7517,7 +7510,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>465</v>
       </c>
@@ -7543,7 +7536,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>585</v>
       </c>
@@ -7560,7 +7553,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" customHeight="1">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>633</v>
       </c>
@@ -7577,7 +7570,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>636</v>
       </c>
@@ -7594,7 +7587,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1">
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>639</v>
       </c>
@@ -7611,7 +7604,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>612</v>
       </c>
@@ -7625,7 +7618,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1">
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>470</v>
       </c>
@@ -7651,7 +7644,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15" customHeight="1">
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>475</v>
       </c>
@@ -7677,7 +7670,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" customHeight="1">
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>591</v>
       </c>
@@ -7691,7 +7684,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" customHeight="1">
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>642</v>
       </c>
@@ -7708,7 +7701,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15" customHeight="1">
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>480</v>
       </c>
@@ -7734,7 +7727,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15" customHeight="1">
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>594</v>
       </c>
@@ -7748,7 +7741,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15" customHeight="1">
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>645</v>
       </c>
@@ -7765,7 +7758,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" customHeight="1">
+    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>588</v>
       </c>
@@ -7779,7 +7772,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" customHeight="1">
+    <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>485</v>
       </c>
@@ -7805,7 +7798,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" customHeight="1">
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>648</v>
       </c>
@@ -7822,7 +7815,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" customHeight="1">
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>651</v>
       </c>
@@ -7839,7 +7832,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" customHeight="1">
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>654</v>
       </c>
@@ -7856,7 +7849,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" customHeight="1">
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>490</v>
       </c>
@@ -7882,7 +7875,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" customHeight="1">
+    <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>600</v>
       </c>
@@ -7896,7 +7889,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" customHeight="1">
+    <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>495</v>
       </c>
@@ -7922,7 +7915,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" customHeight="1">
+    <row r="57" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>500</v>
       </c>
@@ -7948,7 +7941,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" customHeight="1">
+    <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>504</v>
       </c>
@@ -7974,7 +7967,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15" customHeight="1">
+    <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>508</v>
       </c>
@@ -8000,7 +7993,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15" customHeight="1">
+    <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>513</v>
       </c>
@@ -8026,7 +8019,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15" customHeight="1">
+    <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>518</v>
       </c>
@@ -8052,7 +8045,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15" customHeight="1">
+    <row r="62" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>657</v>
       </c>
@@ -8069,7 +8062,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15" customHeight="1">
+    <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>603</v>
       </c>
@@ -8086,7 +8079,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15" customHeight="1">
+    <row r="64" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>522</v>
       </c>
@@ -8112,7 +8105,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15" customHeight="1">
+    <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>660</v>
       </c>
@@ -8129,7 +8122,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="15" customHeight="1">
+    <row r="66" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>527</v>
       </c>
@@ -8146,7 +8139,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15" customHeight="1">
+    <row r="67" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>530</v>
       </c>
@@ -8172,7 +8165,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15" customHeight="1">
+    <row r="68" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>535</v>
       </c>
@@ -8198,7 +8191,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15" customHeight="1">
+    <row r="69" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>539</v>
       </c>
@@ -8224,7 +8217,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15" customHeight="1">
+    <row r="70" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>543</v>
       </c>
@@ -8241,7 +8234,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15" customHeight="1">
+    <row r="71" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>546</v>
       </c>
@@ -8267,7 +8260,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15" customHeight="1">
+    <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>551</v>
       </c>
@@ -8293,7 +8286,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15" customHeight="1">
+    <row r="73" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>663</v>
       </c>
@@ -8310,7 +8303,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15" customHeight="1">
+    <row r="74" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>556</v>
       </c>
@@ -8324,7 +8317,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15" customHeight="1">
+    <row r="75" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>666</v>
       </c>
@@ -8341,7 +8334,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15" customHeight="1">
+    <row r="76" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>559</v>
       </c>
@@ -8358,7 +8351,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15" customHeight="1">
+    <row r="77" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>562</v>
       </c>
@@ -8375,7 +8368,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="15" customHeight="1">
+    <row r="78" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>565</v>
       </c>
@@ -8392,7 +8385,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15" customHeight="1">
+    <row r="79" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>669</v>
       </c>
@@ -8409,7 +8402,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15" customHeight="1">
+    <row r="80" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>672</v>
       </c>
@@ -8426,7 +8419,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15" customHeight="1">
+    <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>568</v>
       </c>
@@ -8452,7 +8445,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15" customHeight="1">
+    <row r="82" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>573</v>
       </c>
@@ -8478,7 +8471,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15" customHeight="1">
+    <row r="83" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>577</v>
       </c>
@@ -8504,7 +8497,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15" customHeight="1">
+    <row r="84" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>582</v>
       </c>
@@ -8521,7 +8514,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15" customHeight="1">
+    <row r="85" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>615</v>
       </c>
@@ -8535,7 +8528,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="15" customHeight="1">
+    <row r="86" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>675</v>
       </c>
@@ -8552,7 +8545,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15" customHeight="1">
+    <row r="87" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>1091</v>
       </c>
@@ -8566,7 +8559,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15" customHeight="1">
+    <row r="88" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>689</v>
       </c>
@@ -8595,7 +8588,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15" customHeight="1">
+    <row r="89" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>692</v>
       </c>
@@ -8624,7 +8617,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15" customHeight="1">
+    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>695</v>
       </c>
@@ -8653,7 +8646,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15" customHeight="1">
+    <row r="91" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>698</v>
       </c>
@@ -8682,7 +8675,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15" customHeight="1">
+    <row r="92" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>701</v>
       </c>
@@ -8711,7 +8704,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15" customHeight="1">
+    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>704</v>
       </c>
@@ -8740,7 +8733,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15" customHeight="1">
+    <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>710</v>
       </c>
@@ -8769,7 +8762,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15" customHeight="1">
+    <row r="95" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>713</v>
       </c>
@@ -8798,7 +8791,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="15" customHeight="1">
+    <row r="96" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>743</v>
       </c>
@@ -8827,7 +8820,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15" customHeight="1">
+    <row r="97" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>716</v>
       </c>
@@ -8856,7 +8849,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="15" customHeight="1">
+    <row r="98" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>719</v>
       </c>
@@ -8885,7 +8878,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15" customHeight="1">
+    <row r="99" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>767</v>
       </c>
@@ -8914,7 +8907,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15" customHeight="1">
+    <row r="100" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>722</v>
       </c>
@@ -8943,7 +8936,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="15" customHeight="1">
+    <row r="101" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>725</v>
       </c>
@@ -8972,7 +8965,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="15" customHeight="1">
+    <row r="102" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>728</v>
       </c>
@@ -9001,7 +8994,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="15" customHeight="1">
+    <row r="103" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>707</v>
       </c>
@@ -9030,7 +9023,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="15" customHeight="1">
+    <row r="104" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>764</v>
       </c>
@@ -9059,7 +9052,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15" customHeight="1">
+    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>731</v>
       </c>
@@ -9088,7 +9081,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="15" customHeight="1">
+    <row r="106" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>734</v>
       </c>
@@ -9117,7 +9110,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15" customHeight="1">
+    <row r="107" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>761</v>
       </c>
@@ -9146,7 +9139,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="15" customHeight="1">
+    <row r="108" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>737</v>
       </c>
@@ -9175,7 +9168,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="15" customHeight="1">
+    <row r="109" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>755</v>
       </c>
@@ -9204,7 +9197,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="15" customHeight="1">
+    <row r="110" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>683</v>
       </c>
@@ -9233,7 +9226,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15" customHeight="1">
+    <row r="111" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>678</v>
       </c>
@@ -9262,7 +9255,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15" customHeight="1">
+    <row r="112" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>686</v>
       </c>
@@ -9291,7 +9284,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15" customHeight="1">
+    <row r="113" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>740</v>
       </c>
@@ -9320,7 +9313,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="15" customHeight="1">
+    <row r="114" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>746</v>
       </c>
@@ -9349,7 +9342,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15" customHeight="1">
+    <row r="115" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>749</v>
       </c>
@@ -9378,7 +9371,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="15" customHeight="1">
+    <row r="116" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>752</v>
       </c>
@@ -9407,7 +9400,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="15" customHeight="1">
+    <row r="117" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>758</v>
       </c>
@@ -9436,7 +9429,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="15" customHeight="1">
+    <row r="118" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>782</v>
       </c>
@@ -9465,7 +9458,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15" customHeight="1">
+    <row r="119" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>786</v>
       </c>
@@ -9494,7 +9487,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="15" customHeight="1">
+    <row r="120" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>790</v>
       </c>
@@ -9523,7 +9516,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15" customHeight="1">
+    <row r="121" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>794</v>
       </c>
@@ -9552,7 +9545,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="15" customHeight="1">
+    <row r="122" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>798</v>
       </c>
@@ -9581,7 +9574,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15" customHeight="1">
+    <row r="123" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>802</v>
       </c>
@@ -9610,7 +9603,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15" customHeight="1">
+    <row r="124" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>810</v>
       </c>
@@ -9639,7 +9632,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="15" customHeight="1">
+    <row r="125" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>814</v>
       </c>
@@ -9668,7 +9661,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="15" customHeight="1">
+    <row r="126" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>854</v>
       </c>
@@ -9697,7 +9690,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="15" customHeight="1">
+    <row r="127" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>818</v>
       </c>
@@ -9726,7 +9719,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="15" customHeight="1">
+    <row r="128" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>822</v>
       </c>
@@ -9755,7 +9748,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15" customHeight="1">
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>886</v>
       </c>
@@ -9784,7 +9777,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="15" customHeight="1">
+    <row r="130" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>826</v>
       </c>
@@ -9813,7 +9806,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="15" customHeight="1">
+    <row r="131" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>830</v>
       </c>
@@ -9842,7 +9835,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="15" customHeight="1">
+    <row r="132" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>834</v>
       </c>
@@ -9871,7 +9864,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="15" customHeight="1">
+    <row r="133" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>806</v>
       </c>
@@ -9900,7 +9893,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="15" customHeight="1">
+    <row r="134" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>882</v>
       </c>
@@ -9929,7 +9922,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="15" customHeight="1">
+    <row r="135" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>838</v>
       </c>
@@ -9958,7 +9951,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15" customHeight="1">
+    <row r="136" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>842</v>
       </c>
@@ -9987,7 +9980,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="15" customHeight="1">
+    <row r="137" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>878</v>
       </c>
@@ -10016,7 +10009,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15" customHeight="1">
+    <row r="138" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>846</v>
       </c>
@@ -10045,7 +10038,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15" customHeight="1">
+    <row r="139" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>870</v>
       </c>
@@ -10074,7 +10067,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15" customHeight="1">
+    <row r="140" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>774</v>
       </c>
@@ -10103,7 +10096,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15" customHeight="1">
+    <row r="141" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>770</v>
       </c>
@@ -10132,7 +10125,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15" customHeight="1">
+    <row r="142" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>778</v>
       </c>
@@ -10161,7 +10154,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15" customHeight="1">
+    <row r="143" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>850</v>
       </c>
@@ -10190,7 +10183,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15" customHeight="1">
+    <row r="144" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>858</v>
       </c>
@@ -10219,7 +10212,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="15" customHeight="1">
+    <row r="145" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>862</v>
       </c>
@@ -10248,7 +10241,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="15" customHeight="1">
+    <row r="146" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>866</v>
       </c>
@@ -10277,7 +10270,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="15" customHeight="1">
+    <row r="147" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>874</v>
       </c>
@@ -10306,7 +10299,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="15" customHeight="1">
+    <row r="148" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>903</v>
       </c>
@@ -10335,7 +10328,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="15" customHeight="1">
+    <row r="149" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>907</v>
       </c>
@@ -10364,7 +10357,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="15" customHeight="1">
+    <row r="150" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>911</v>
       </c>
@@ -10393,7 +10386,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="15" customHeight="1">
+    <row r="151" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>915</v>
       </c>
@@ -10422,7 +10415,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="15" customHeight="1">
+    <row r="152" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>919</v>
       </c>
@@ -10451,7 +10444,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="15" customHeight="1">
+    <row r="153" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>923</v>
       </c>
@@ -10480,7 +10473,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="15" customHeight="1">
+    <row r="154" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>931</v>
       </c>
@@ -10509,7 +10502,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="15" customHeight="1">
+    <row r="155" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>935</v>
       </c>
@@ -10538,7 +10531,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="15" customHeight="1">
+    <row r="156" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>975</v>
       </c>
@@ -10567,7 +10560,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="15" customHeight="1">
+    <row r="157" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>939</v>
       </c>
@@ -10596,7 +10589,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="15" customHeight="1">
+    <row r="158" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>943</v>
       </c>
@@ -10625,7 +10618,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="15" customHeight="1">
+    <row r="159" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>1007</v>
       </c>
@@ -10654,7 +10647,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="15" customHeight="1">
+    <row r="160" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>947</v>
       </c>
@@ -10683,7 +10676,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="15" customHeight="1">
+    <row r="161" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>951</v>
       </c>
@@ -10712,7 +10705,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="15" customHeight="1">
+    <row r="162" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>955</v>
       </c>
@@ -10741,7 +10734,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15" customHeight="1">
+    <row r="163" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>927</v>
       </c>
@@ -10770,7 +10763,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="15" customHeight="1">
+    <row r="164" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>1003</v>
       </c>
@@ -10799,7 +10792,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15" customHeight="1">
+    <row r="165" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>959</v>
       </c>
@@ -10828,7 +10821,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15" customHeight="1">
+    <row r="166" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>963</v>
       </c>
@@ -10857,7 +10850,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15" customHeight="1">
+    <row r="167" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>999</v>
       </c>
@@ -10886,7 +10879,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15" customHeight="1">
+    <row r="168" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>967</v>
       </c>
@@ -10915,7 +10908,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15" customHeight="1">
+    <row r="169" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>991</v>
       </c>
@@ -10944,7 +10937,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15" customHeight="1">
+    <row r="170" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>895</v>
       </c>
@@ -10973,7 +10966,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15" customHeight="1">
+    <row r="171" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>890</v>
       </c>
@@ -11002,7 +10995,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15" customHeight="1">
+    <row r="172" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>899</v>
       </c>
@@ -11031,7 +11024,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15" customHeight="1">
+    <row r="173" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>971</v>
       </c>
@@ -11060,7 +11053,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15" customHeight="1">
+    <row r="174" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>979</v>
       </c>
@@ -11089,7 +11082,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15" customHeight="1">
+    <row r="175" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>983</v>
       </c>
@@ -11118,7 +11111,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15" customHeight="1">
+    <row r="176" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>987</v>
       </c>
@@ -11147,7 +11140,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="15" customHeight="1">
+    <row r="177" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>995</v>
       </c>
@@ -11184,11 +11177,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11203,7 +11191,7 @@
       <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" style="3" bestFit="1" customWidth="1"/>
@@ -11214,7 +11202,7 @@
     <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="str">
         <f>Submodels!$A$1</f>
         <v>ID</v>
@@ -11235,7 +11223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1013</v>
       </c>
@@ -11249,7 +11237,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1016</v>
       </c>
@@ -11263,7 +11251,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1018</v>
       </c>
@@ -11283,7 +11271,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1022</v>
       </c>
@@ -11303,7 +11291,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1025</v>
       </c>
@@ -11323,11 +11311,6 @@
   </sheetData>
   <autoFilter ref="A1:F6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11342,7 +11325,7 @@
       <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
@@ -11351,7 +11334,7 @@
     <col min="6" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="30" customHeight="1">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11368,7 +11351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1029</v>
       </c>
@@ -11382,7 +11365,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1033</v>
       </c>
@@ -11396,7 +11379,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1036</v>
       </c>
@@ -11413,7 +11396,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1040</v>
       </c>
@@ -11427,7 +11410,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1043</v>
       </c>
@@ -11441,7 +11424,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>1046</v>
       </c>
@@ -11455,7 +11438,7 @@
         <v>815332823</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1049</v>
       </c>
@@ -11469,7 +11452,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1052</v>
       </c>
@@ -11483,7 +11466,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1055</v>
       </c>
@@ -11497,7 +11480,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1058</v>
       </c>
@@ -11511,7 +11494,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1061</v>
       </c>
@@ -11525,7 +11508,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1064</v>
       </c>
@@ -11539,7 +11522,7 @@
         <v>33184</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1067</v>
       </c>
@@ -11553,7 +11536,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1068</v>
       </c>
@@ -11567,7 +11550,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>1069</v>
       </c>
@@ -11581,7 +11564,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>1070</v>
       </c>
@@ -11595,7 +11578,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>1071</v>
       </c>
@@ -11609,7 +11592,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>1072</v>
       </c>
@@ -11623,7 +11606,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>1073</v>
       </c>
@@ -11640,10 +11623,5 @@
   </sheetData>
   <autoFilter ref="A1:E20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>